<commit_message>
modified naming + solved leaders in array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1711,8 +1711,8 @@
   </sheetPr>
   <dimension ref="A1:C658"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1785,13 +1785,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added union of 2 arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1712,7 +1712,7 @@
   <dimension ref="A1:C658"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1807,13 +1807,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added rotate array by one position
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1712,7 +1712,7 @@
   <dimension ref="A1:C658"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1818,13 +1818,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solved find duplicates in array + working on min jumps + modified templates
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1712,7 +1712,7 @@
   <dimension ref="A1:C658"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1851,13 +1851,13 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="14" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added 0-1 knapsack top down
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1711,8 +1711,8 @@
   </sheetPr>
   <dimension ref="A1:C658"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A392" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B418" activeCellId="0" sqref="B418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1862,13 +1862,13 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -6055,13 +6055,13 @@
       </c>
     </row>
     <row r="411" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="10" t="s">
+      <c r="A411" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="B411" s="11" t="s">
+      <c r="B411" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="C411" s="6" t="s">
+      <c r="C411" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added GFG: Common elements
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1711,8 +1711,8 @@
   </sheetPr>
   <dimension ref="A1:C658"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A392" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B418" activeCellId="0" sqref="B418"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1928,24 +1928,24 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="14" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added gfg: Smallest Positive missing number
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1711,8 +1711,8 @@
   </sheetPr>
   <dimension ref="A1:C658"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1884,13 +1884,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1939,24 +1939,24 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>